<commit_message>
Añadir fichero de actualizacion de los anuarios estadísticos
</commit_message>
<xml_diff>
--- a/Datos/Anuario2024/020701_MFTMNP.xlsx
+++ b/Datos/Anuario2024/020701_MFTMNP.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Tomas\AplAnu2024\System\Xls_Cast\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8715" tabRatio="779" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8715" tabRatio="779"/>
   </bookViews>
   <sheets>
-    <sheet name="0" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="0" sheetId="190" r:id="rId1"/>
+    <sheet name="1" sheetId="119" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -95,57 +101,84 @@
     <definedName name="p">'[2]4.27'!$A$1:$G$22</definedName>
     <definedName name="u">'[2]4.17'!$A$1:$I$8</definedName>
   </definedNames>
-  <calcPr calcId="152511" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId253" roundtripDataSignature="AMtx7mizkmFRPNryej4reDhSC2xgXklycg=="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Mujeres</t>
+  </si>
+  <si>
+    <t>MUERTES FETALES TARDÍAS</t>
+  </si>
+  <si>
+    <t>Hombres</t>
+  </si>
+  <si>
+    <t>Fuente: Movimiento Natural de la Población. INE.</t>
+  </si>
+  <si>
+    <t>1. Muertes fetales tardías según sexo. 2022</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <color theme="1"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <b val="1"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="10"/>
     </font>
     <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <i val="1"/>
-      <color theme="1"/>
-      <sz val="8"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -174,102 +207,43 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="1"/>
       <sheetName val="1.1"/>
@@ -428,8 +402,8 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook r:id="rId1">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="1"/>
       <sheetName val="1.1"/>
@@ -1336,124 +1310,96 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col width="35.7109375" customWidth="1" min="1" max="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="7" t="inlineStr">
-        <is>
-          <t>MUERTES FETALES TARDÍAS</t>
-        </is>
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>2</v>
       </c>
-      <c r="B1" s="1" t="n"/>
+      <c r="B1" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.3937007874015748" right="0.3937007874015748" top="0.5905511811023622" bottom="0.5905511811023622" header="0" footer="0"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.39370078740157477" right="0.39370078740157477" top="0.59055118110236215" bottom="0.59055118110236215" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Times New Roman,Normal"&amp;9 Oficina d'Estadística&amp;R&amp;"Times New Roman,Normal"&amp;9 Ajuntament de València</oddHeader>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
+    <oddHeader>&amp;L&amp;"Times New Roman,Normal"&amp;9Oficina d'Estadística&amp;R&amp;"Times New Roman,Normal"&amp;9Ajuntament de València</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="7" t="inlineStr">
-        <is>
-          <t>1. Muertes fetales tardías según sexo. 2022</t>
-        </is>
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
       </c>
-      <c r="B1" s="4" t="n"/>
-      <c r="C1" s="2" t="n"/>
-      <c r="D1" s="1" t="n"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="1"/>
     </row>
-    <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="4" t="n"/>
-      <c r="B2" s="4" t="n"/>
-      <c r="C2" s="2" t="n"/>
-      <c r="D2" s="1" t="n"/>
+    <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1"/>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="5" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
       </c>
-      <c r="B3" s="5" t="inlineStr">
-        <is>
-          <t>Hombres</t>
-        </is>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
       </c>
-      <c r="C3" s="5" t="inlineStr">
-        <is>
-          <t>Mujeres</t>
-        </is>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
       </c>
-      <c r="D3" s="1" t="n"/>
+      <c r="D3" s="1"/>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="2" t="n">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="2">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="2">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="n"/>
+      <c r="D4" s="1"/>
     </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="3" t="inlineStr">
-        <is>
-          <t>Fuente: Movimiento Natural de la Población. INE.</t>
-        </is>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
       </c>
-      <c r="B5" s="6" t="n"/>
-      <c r="C5" s="1" t="n"/>
-      <c r="D5" s="1" t="n"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.3937007874015748" right="0.3937007874015748" top="0.5905511811023622" bottom="0.5905511811023622" header="0" footer="0"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.39370078740157477" right="0.39370078740157477" top="0.59055118110236215" bottom="0.59055118110236215" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Times New Roman,Normal"&amp;9 Oficina d'Estadística&amp;R&amp;"Times New Roman,Normal"&amp;9 Ajuntament de València</oddHeader>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
+    <oddHeader>&amp;L&amp;"Times New Roman,Normal"&amp;9Oficina d'Estadística&amp;R&amp;"Times New Roman,Normal"&amp;9Ajuntament de València</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>